<commit_message>
Add key investor options
</commit_message>
<xml_diff>
--- a/public/templates/stocks_template.xlsx
+++ b/public/templates/stocks_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benab\OneDrive - iitkgp.ac.in\Desktop\WebDev\GameOfTrades\stocksimulator\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D006502B-7E4B-485C-BFDF-4BBA65FE9C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38111EC4-7984-4F2E-B09C-771A5B383D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Symbol</t>
   </si>
@@ -48,30 +48,89 @@
     <t>Volatility Factor</t>
   </si>
   <si>
-    <t>HDFC</t>
-  </si>
-  <si>
-    <t>HDFC Bank</t>
-  </si>
-  <si>
     <t>Banking</t>
   </si>
   <si>
-    <t>A banking sample stock</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
     <t>Current Price</t>
+  </si>
+  <si>
+    <t>INFY</t>
+  </si>
+  <si>
+    <t>Infosys Ltd.</t>
+  </si>
+  <si>
+    <t>IT Services</t>
+  </si>
+  <si>
+    <t>Leading IT consulting and outsourcing firm</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>RELI</t>
+  </si>
+  <si>
+    <t>Reliance Ind.</t>
+  </si>
+  <si>
+    <t>Conglomerate</t>
+  </si>
+  <si>
+    <t>Diversified biz in energy, retail, telecom</t>
+  </si>
+  <si>
+    <t>TCS</t>
+  </si>
+  <si>
+    <t>Tata Consultancy</t>
+  </si>
+  <si>
+    <t>Top global IT services and consulting firm</t>
+  </si>
+  <si>
+    <t>ICIC</t>
+  </si>
+  <si>
+    <t>ICICI Bank</t>
+  </si>
+  <si>
+    <t>Major private sector bank in India</t>
+  </si>
+  <si>
+    <t>DMART</t>
+  </si>
+  <si>
+    <t>Avenue Supermarts</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>Operates D-Mart chain across India</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -99,8 +158,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,64 +446,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1450</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2">
+        <v>100</v>
+      </c>
+      <c r="H2" s="2">
+        <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2750</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2">
+        <v>150</v>
+      </c>
+      <c r="H3" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3600</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2">
+        <v>100</v>
+      </c>
+      <c r="H4" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1120</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>1500</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
-      </c>
-      <c r="H2">
-        <v>50</v>
+      <c r="G5" s="2">
+        <v>75</v>
+      </c>
+      <c r="H5" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4100</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="2">
+        <v>200</v>
+      </c>
+      <c r="H6" s="2">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>